<commit_message>
prevent true false string becoming boolean
</commit_message>
<xml_diff>
--- a/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/control_stubs.xlsx
+++ b/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/control_stubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joehasell/Documents/OWID/notebooks/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{79E5EFBC-9472-444C-ABF0-56D8CB552AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7646F4B0-B55E-B74A-8182-D5459A12500A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36120" yWindow="3520" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{376489E3-129A-9E4B-A657-B41146175634}"/>
   </bookViews>
@@ -286,12 +286,6 @@
     <t>[welfare$radio_option]</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>table_slug_suffix</t>
   </si>
   <si>
@@ -308,6 +302,12 @@
   </si>
   <si>
     <t>_extrap</t>
+  </si>
+  <si>
+    <t>'true</t>
+  </si>
+  <si>
+    <t>'false</t>
   </si>
 </sst>
 </file>
@@ -780,10 +780,10 @@
         <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>81</v>
@@ -841,10 +841,10 @@
         <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>81</v>
@@ -898,10 +898,10 @@
         <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>81</v>
@@ -959,10 +959,10 @@
         <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>81</v>
@@ -1020,10 +1020,10 @@
         <v>65</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>81</v>
@@ -1081,10 +1081,10 @@
         <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>81</v>
@@ -36093,7 +36093,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36104,26 +36104,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="B3" t="s">
         <v>83</v>
-      </c>
-      <c r="B3" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Typo in control stubs and add derived variables
</commit_message>
<xml_diff>
--- a/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/control_stubs.xlsx
+++ b/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/control_stubs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joehasell/Documents/OWID/notebooks/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{9C62E7B7-A765-5F42-BE3A-0E7BDD272874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E8BE0FCE-1520-9F4C-B6AE-0A5EA394704B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36120" yWindow="3520" windowWidth="28040" windowHeight="17440" xr2:uid="{376489E3-129A-9E4B-A657-B41146175634}"/>
+    <workbookView xWindow="36100" yWindow="3500" windowWidth="28040" windowHeight="17440" xr2:uid="{376489E3-129A-9E4B-A657-B41146175634}"/>
   </bookViews>
   <sheets>
     <sheet name="control_stubs" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
   </si>
   <si>
     <t>subtitle</t>
-  </si>
-  <si>
-    <t>notes</t>
   </si>
   <si>
     <t>sourceName</t>
@@ -262,9 +259,6 @@
     <t>Poverty: Number of people living on less than $[abs_povline$text] a day</t>
   </si>
   <si>
-    <t>Poverty gap index at $[abs_povline$text] a day.</t>
-  </si>
-  <si>
     <t>Depth of poverty: Average percentage shortfall of [welfare$text] below $[abs_povline$text] a day</t>
   </si>
   <si>
@@ -317,6 +311,12 @@
   </si>
   <si>
     <t>Numeric</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Poverty gap index at $[abs_povline$text] a day</t>
   </si>
 </sst>
 </file>
@@ -711,7 +711,7 @@
   <dimension ref="A1:AF1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -738,10 +738,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
@@ -750,16 +750,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>1</v>
@@ -768,10 +768,10 @@
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -793,49 +793,49 @@
     </row>
     <row r="2" spans="1:32" ht="43" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N2" s="3">
         <v>0</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -857,45 +857,45 @@
     </row>
     <row r="3" spans="1:32" ht="43" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N3" s="3">
         <v>0</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
@@ -916,49 +916,49 @@
     </row>
     <row r="4" spans="1:32" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="L4" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N4" s="3">
         <v>0</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -980,49 +980,49 @@
     </row>
     <row r="5" spans="1:32" ht="71" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="K5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N5" s="3">
         <v>0</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -1044,49 +1044,49 @@
     </row>
     <row r="6" spans="1:32" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>60</v>
+      <c r="H6" s="3" t="s">
+        <v>18</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>81</v>
+      <c r="I6" s="3" t="s">
+        <v>13</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="L6" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N6" s="3">
         <v>0</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -1108,49 +1108,49 @@
     </row>
     <row r="7" spans="1:32" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="H7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="K7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N7" s="3">
         <v>0</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
@@ -34949,21 +34949,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -34971,10 +34971,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>1.9</v>
@@ -34982,10 +34982,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>3.2</v>
@@ -34993,10 +34993,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>5.5</v>
@@ -35004,10 +35004,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -35015,10 +35015,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7">
         <v>15</v>
@@ -35026,10 +35026,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -35037,10 +35037,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9">
         <v>30</v>
@@ -35048,10 +35048,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <v>40</v>
@@ -35081,46 +35081,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>50</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>54</v>
       </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -35144,26 +35144,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing small change to controls
</commit_message>
<xml_diff>
--- a/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/control_stubs.xlsx
+++ b/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/control_stubs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joehasell/Documents/OWID/notebooks/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E86869-308A-5A4B-BFF6-0B5D501E68DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3CD5AB-63A7-7842-85FD-9E50D2B190B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36100" yWindow="3500" windowWidth="28040" windowHeight="17440" xr2:uid="{376489E3-129A-9E4B-A657-B41146175634}"/>
   </bookViews>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>shortUnit</t>
-  </si>
-  <si>
-    <t>Share in poverty</t>
   </si>
   <si>
     <t>This data is adjusted for differences in the cost of living between countries and for inflation.</t>
@@ -317,6 +314,9 @@
   </si>
   <si>
     <t>Poverty gap index at $[abs_povline$text] a day</t>
+  </si>
+  <si>
+    <t>Share in povertyX</t>
   </si>
 </sst>
 </file>
@@ -711,7 +711,7 @@
   <dimension ref="A1:AF1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -738,10 +738,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
@@ -750,7 +750,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
@@ -768,10 +768,10 @@
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -793,49 +793,49 @@
     </row>
     <row r="2" spans="1:32" ht="43" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="K2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N2" s="3">
         <v>0</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -857,45 +857,45 @@
     </row>
     <row r="3" spans="1:32" ht="43" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N3" s="3">
         <v>0</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
@@ -916,49 +916,49 @@
     </row>
     <row r="4" spans="1:32" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L4" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N4" s="3">
         <v>0</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -980,49 +980,49 @@
     </row>
     <row r="5" spans="1:32" ht="71" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="H5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="K5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N5" s="3">
         <v>0</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -1044,49 +1044,49 @@
     </row>
     <row r="6" spans="1:32" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>59</v>
+      <c r="H6" s="3" t="s">
+        <v>17</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>79</v>
+      <c r="I6" s="3" t="s">
+        <v>12</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="L6" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N6" s="3">
         <v>0</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -1108,49 +1108,49 @@
     </row>
     <row r="7" spans="1:32" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="H7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="K7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N7" s="3">
         <v>0</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
@@ -34949,21 +34949,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -34971,10 +34971,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>1.9</v>
@@ -34982,10 +34982,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>3.2</v>
@@ -34993,10 +34993,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5">
         <v>5.5</v>
@@ -35004,10 +35004,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -35015,10 +35015,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7">
         <v>15</v>
@@ -35026,10 +35026,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -35037,10 +35037,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9">
         <v>30</v>
@@ -35048,10 +35048,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10">
         <v>40</v>
@@ -35082,46 +35082,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>49</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>53</v>
       </c>
-      <c r="C3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -35145,26 +35145,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing small change take 2
</commit_message>
<xml_diff>
--- a/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/control_stubs.xlsx
+++ b/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/control_stubs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joehasell/Documents/OWID/notebooks/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3CD5AB-63A7-7842-85FD-9E50D2B190B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C72CB7D-19B7-6043-BD7C-819C7F30B441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36100" yWindow="3500" windowWidth="28040" windowHeight="17440" xr2:uid="{376489E3-129A-9E4B-A657-B41146175634}"/>
+    <workbookView xWindow="37240" yWindow="3620" windowWidth="28040" windowHeight="17440" xr2:uid="{376489E3-129A-9E4B-A657-B41146175634}"/>
   </bookViews>
   <sheets>
     <sheet name="control_stubs" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Undoing small change for test
</commit_message>
<xml_diff>
--- a/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/control_stubs.xlsx
+++ b/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/control_stubs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joehasell/Documents/OWID/notebooks/JoeHasell/Povcal_data_work/Povcal_PIP_explorer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C72CB7D-19B7-6043-BD7C-819C7F30B441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C69417A-873D-9041-802A-D35D7FA93E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37240" yWindow="3620" windowWidth="28040" windowHeight="17440" xr2:uid="{376489E3-129A-9E4B-A657-B41146175634}"/>
   </bookViews>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>shortUnit</t>
+  </si>
+  <si>
+    <t>Share in poverty</t>
   </si>
   <si>
     <t>This data is adjusted for differences in the cost of living between countries and for inflation.</t>
@@ -314,9 +317,6 @@
   </si>
   <si>
     <t>Poverty gap index at $[abs_povline$text] a day</t>
-  </si>
-  <si>
-    <t>Share in povertyX</t>
   </si>
 </sst>
 </file>
@@ -738,10 +738,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
@@ -750,7 +750,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>7</v>
@@ -768,10 +768,10 @@
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -793,49 +793,49 @@
     </row>
     <row r="2" spans="1:32" ht="43" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="N2" s="3">
         <v>0</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -857,45 +857,45 @@
     </row>
     <row r="3" spans="1:32" ht="43" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N3" s="3">
         <v>0</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
@@ -916,49 +916,49 @@
     </row>
     <row r="4" spans="1:32" ht="57" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N4" s="3">
         <v>0</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -980,49 +980,49 @@
     </row>
     <row r="5" spans="1:32" ht="71" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N5" s="3">
         <v>0</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -1044,49 +1044,49 @@
     </row>
     <row r="6" spans="1:32" ht="57" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N6" s="3">
         <v>0</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
@@ -1108,49 +1108,49 @@
     </row>
     <row r="7" spans="1:32" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N7" s="3">
         <v>0</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
@@ -34949,21 +34949,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>26</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -34971,10 +34971,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>1.9</v>
@@ -34982,10 +34982,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>3.2</v>
@@ -34993,10 +34993,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>5.5</v>
@@ -35004,10 +35004,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -35015,10 +35015,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7">
         <v>15</v>
@@ -35026,10 +35026,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -35037,10 +35037,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9">
         <v>30</v>
@@ -35048,10 +35048,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10">
         <v>40</v>
@@ -35082,46 +35082,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="B4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -35145,26 +35145,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>